<commit_message>
FEC done except converting to last name string
</commit_message>
<xml_diff>
--- a/FEC/fec_crosswalk.xlsx
+++ b/FEC/fec_crosswalk.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andrew/OneDrive/Galvanize/Capstone/git/election_predictions/FEC/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB0CB8ED-4D7F-6945-AE45-D2D671BBF8E5}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6373283A-3D2B-E742-8594-F9BBEEE8BE63}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1380" yWindow="460" windowWidth="26440" windowHeight="16520" xr2:uid="{85084A1C-5921-824E-8042-478A2AEBFF16}"/>
+    <workbookView xWindow="180" yWindow="460" windowWidth="18960" windowHeight="16520" xr2:uid="{85084A1C-5921-824E-8042-478A2AEBFF16}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
     <t>CCL</t>
   </si>
@@ -106,6 +106,30 @@
   </si>
   <si>
     <t>Committee contributions to candidates</t>
+  </si>
+  <si>
+    <t>millions x 21</t>
+  </si>
+  <si>
+    <t>7643 x 15</t>
+  </si>
+  <si>
+    <t>PAS2_TRANS</t>
+  </si>
+  <si>
+    <t>INDIV_TRANS</t>
+  </si>
+  <si>
+    <t>PAS2 trans. grouped by CMTE_ID</t>
+  </si>
+  <si>
+    <t>INDIV trans. grouped by CMTE_ID</t>
+  </si>
+  <si>
+    <t>6235 x 2</t>
+  </si>
+  <si>
+    <t>Transactions from PAS2 and CCL grouped by CMTE_ID</t>
   </si>
 </sst>
 </file>
@@ -145,7 +169,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -179,6 +203,17 @@
       </left>
       <right/>
       <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
       <bottom/>
       <diagonal/>
     </border>
@@ -308,62 +343,87 @@
       </right>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -680,23 +740,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F843C19-ED32-EA45-A124-E5AA1582ACC4}">
-  <dimension ref="A1:G17"/>
+  <dimension ref="A1:I17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="23.1640625" customWidth="1"/>
-    <col min="2" max="2" width="18.33203125" style="9" customWidth="1"/>
-    <col min="3" max="4" width="18.33203125" style="10" customWidth="1"/>
-    <col min="5" max="5" width="18.33203125" style="11" customWidth="1"/>
-    <col min="6" max="6" width="18.33203125" style="10" customWidth="1"/>
-    <col min="7" max="7" width="16.83203125" customWidth="1"/>
+    <col min="2" max="2" width="15.5" style="9" customWidth="1"/>
+    <col min="3" max="4" width="15.5" style="10" customWidth="1"/>
+    <col min="5" max="5" width="15.5" style="11" customWidth="1"/>
+    <col min="6" max="7" width="15.5" style="22" customWidth="1"/>
+    <col min="8" max="8" width="15.5" style="10" customWidth="1"/>
+    <col min="9" max="9" width="16.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="19" x14ac:dyDescent="0.25">
       <c r="B1" s="14" t="s">
         <v>18</v>
       </c>
@@ -705,8 +766,10 @@
       <c r="E1" s="15"/>
       <c r="F1" s="15"/>
       <c r="G1" s="15"/>
-    </row>
-    <row r="2" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
+    </row>
+    <row r="2" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B2" s="5" t="s">
         <v>0</v>
       </c>
@@ -719,11 +782,17 @@
       <c r="E2" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="F2" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="G2" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="H2" s="6" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:7" s="1" customFormat="1" ht="48" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" s="1" customFormat="1" ht="64" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>20</v>
       </c>
@@ -739,9 +808,17 @@
       <c r="E3" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="F3" s="12"/>
-    </row>
-    <row r="4" spans="1:7" s="2" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="F3" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="G3" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="H3" s="12" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" s="2" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>17</v>
       </c>
@@ -751,66 +828,105 @@
       <c r="C4" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="D4" s="17"/>
-      <c r="E4" s="18"/>
-      <c r="F4" s="17"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D4" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="E4" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="F4" s="21">
+        <v>4993</v>
+      </c>
+      <c r="G4" s="21">
+        <v>4263</v>
+      </c>
+      <c r="H4" s="17" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B5" s="9">
+        <v>5884</v>
+      </c>
+      <c r="C5" s="10">
+        <v>1699</v>
+      </c>
+      <c r="E5" s="11">
+        <v>7643</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B6" s="9">
+        <v>6270</v>
+      </c>
+      <c r="C6" s="10">
+        <v>4993</v>
+      </c>
+      <c r="D6" s="10">
+        <v>4263</v>
+      </c>
+      <c r="F6" s="22">
+        <v>4993</v>
+      </c>
+      <c r="G6" s="22">
+        <v>4263</v>
+      </c>
+      <c r="H6" s="10">
+        <v>6235</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>13</v>
       </c>
@@ -822,7 +938,7 @@
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B1:G1"/>
+    <mergeCell ref="B1:I1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>